<commit_message>
change in salary made
</commit_message>
<xml_diff>
--- a/File data.xlsx
+++ b/File data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -449,7 +449,7 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>55000</v>
+        <v>55070</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>